<commit_message>
attempt to save movement plots as pdf in each chunk
</commit_message>
<xml_diff>
--- a/results_NEB/06_distance_LitoLi_intratriad_litype4.xlsx
+++ b/results_NEB/06_distance_LitoLi_intratriad_litype4.xlsx
@@ -104,8 +104,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -146,7 +147,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +158,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF6F9D4"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FF99CCFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -201,7 +208,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -215,6 +222,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -243,7 +254,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -298,10 +309,10 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="topLeft" activeCell="K24" activeCellId="0" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="n">
@@ -1724,7 +1735,7 @@
         <f aca="false">SQRT(SUMSQ(I2:I25)/COUNT(I2:I25))</f>
         <v>0.510757932068444</v>
       </c>
-      <c r="J27" s="3" t="n">
+      <c r="J27" s="4" t="n">
         <f aca="false">SQRT(SUMSQ(J2:J25)/COUNT(J2:J25))</f>
         <v>0.371233065326442</v>
       </c>

</xml_diff>